<commit_message>
Update to jellyfish stats spreadsheet
</commit_message>
<xml_diff>
--- a/python/jellyfish_stats.xlsx
+++ b/python/jellyfish_stats.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\apps\hm-bit-count-decoder\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onsmi\Documents\apps\hm-bit-count-decoder\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12214"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,6 +105,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -478,6 +479,472 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prediction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$42:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5542941.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1483772.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>811175.125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>603595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-56A4-4D69-9EFC-91947BD6E695}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>residual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$42:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11813752.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1849526.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>795704.625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>381760.625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-56A4-4D69-9EFC-91947BD6E695}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$42:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>906505.125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>374579</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>275522.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120680.375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-56A4-4D69-9EFC-91947BD6E695}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="349940640"/>
+        <c:axId val="349940968"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="349940640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="349940968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="349940968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="349940640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -584,8 +1051,553 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1122,6 +2134,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>585105</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>106134</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>244928</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>48985</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1427,13 +2469,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D11"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="12" bestFit="1" customWidth="1"/>
@@ -1441,7 +2483,7 @@
     <col min="7" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1467,7 +2509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>363976743</v>
       </c>
@@ -1481,19 +2523,19 @@
         <v>1742182.375</v>
       </c>
       <c r="F2">
-        <v>73105843</v>
+        <v>18263199</v>
       </c>
       <c r="G2">
-        <v>12995767</v>
+        <v>5542941.625</v>
       </c>
       <c r="H2">
-        <v>58402392.875</v>
+        <v>11813752.25</v>
       </c>
       <c r="I2">
-        <v>1707683.125</v>
+        <v>906505.125</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>289970358</v>
       </c>
@@ -1507,19 +2549,19 @@
         <v>1846351.125</v>
       </c>
       <c r="F3">
-        <v>36544663</v>
+        <v>3707878</v>
       </c>
       <c r="G3">
-        <v>8831983.125</v>
+        <v>1483772.25</v>
       </c>
       <c r="H3">
-        <v>26407419.875</v>
+        <v>1849526.75</v>
       </c>
       <c r="I3">
-        <v>1305260</v>
+        <v>374579</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>217022706</v>
       </c>
@@ -1533,19 +2575,19 @@
         <v>1943655.375</v>
       </c>
       <c r="F4">
-        <v>18263199</v>
+        <v>1882402</v>
       </c>
       <c r="G4">
-        <v>5542941.625</v>
+        <v>811175.125</v>
       </c>
       <c r="H4">
-        <v>11813752.25</v>
+        <v>795704.625</v>
       </c>
       <c r="I4">
-        <v>906505.125</v>
+        <v>275522.25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>144913374</v>
       </c>
@@ -1559,19 +2601,19 @@
         <v>1946296.375</v>
       </c>
       <c r="F5">
-        <v>3707878</v>
+        <v>1106036</v>
       </c>
       <c r="G5">
-        <v>1483772.25</v>
+        <v>603595</v>
       </c>
       <c r="H5">
-        <v>1849526.75</v>
+        <v>381760.625</v>
       </c>
       <c r="I5">
-        <v>374579</v>
+        <v>120680.375</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>73105843</v>
       </c>
@@ -1584,20 +2626,8 @@
       <c r="D6">
         <v>1707683.125</v>
       </c>
-      <c r="F6">
-        <v>1882402</v>
-      </c>
-      <c r="G6">
-        <v>811175.125</v>
-      </c>
-      <c r="H6">
-        <v>795704.625</v>
-      </c>
-      <c r="I6">
-        <v>275522.25</v>
-      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>36544663</v>
       </c>
@@ -1610,20 +2640,8 @@
       <c r="D7">
         <v>1305260</v>
       </c>
-      <c r="F7">
-        <v>1106036</v>
-      </c>
-      <c r="G7">
-        <v>603595</v>
-      </c>
-      <c r="H7">
-        <v>381760.625</v>
-      </c>
-      <c r="I7">
-        <v>120680.375</v>
-      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>18263199</v>
       </c>
@@ -1637,7 +2655,7 @@
         <v>906505.125</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>3707878</v>
       </c>
@@ -1651,7 +2669,7 @@
         <v>374579</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1882402</v>
       </c>
@@ -1665,7 +2683,7 @@
         <v>275522.25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>1106036</v>
       </c>
@@ -1677,6 +2695,26 @@
       </c>
       <c r="D11">
         <v>120680.375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A45">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jellyfish stats are correct now
</commit_message>
<xml_diff>
--- a/python/jellyfish_stats.xlsx
+++ b/python/jellyfish_stats.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onsmi\Documents\apps\hm-bit-count-decoder\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\apps\hm-bit-count-decoder\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12214"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,18 +24,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>total</t>
   </si>
   <si>
-    <t>prediction</t>
+    <t>target_bitrate_kbps</t>
   </si>
   <si>
-    <t>residual</t>
+    <t>achieved_bitrate_kbps</t>
   </si>
   <si>
-    <t>other</t>
+    <t>prediction_kbps</t>
+  </si>
+  <si>
+    <t>residual_kbps</t>
+  </si>
+  <si>
+    <t>other_kbps</t>
+  </si>
+  <si>
+    <t>avg_psnr</t>
+  </si>
+  <si>
+    <t>avg_qp</t>
   </si>
 </sst>
 </file>
@@ -105,7 +117,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -147,11 +158,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>prediction</c:v>
+                  <c:v>prediction_kbps</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -166,48 +177,87 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>21653017.5</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21864241.625</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20674481.75</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17901690.5</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12995767</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8831983.125</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5542941.625</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1483772.25</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>811175.125</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>603595</c:v>
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5768.3638620000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5824.6339688999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5507.6819381999903</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4769.0103491999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3462.0723287999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2352.8403045</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1476.6396489000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>395.27692739999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>216.0970533</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160.797708</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1FA6-43D9-8641-4895429DF0A7}"/>
+              <c16:uniqueId val="{00000000-EAEE-4C7D-BF3B-696838ED774A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -216,11 +266,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>residual</c:v>
+                  <c:v>residual_kbps</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -235,48 +285,87 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>340581543.125</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>266259765.25</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>194404568.875</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>125065387.125</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>58402392.875</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26407419.875</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11813752.25</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1849526.75</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>795704.625</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>381760.625</c:v>
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>90730.9230885</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70931.601462599996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51789.377148300002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33317.419130099901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15558.3974619</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7034.9366547</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3147.1835993999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>492.7139262</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>211.97571209999899</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>101.7010305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1FA6-43D9-8641-4895429DF0A7}"/>
+              <c16:uniqueId val="{00000001-EAEE-4C7D-BF3B-696838ED774A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -285,11 +374,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>other</c:v>
+                  <c:v>other_kbps</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -304,48 +393,87 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1742182.375</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1846351.125</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1943655.375</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1946296.375</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1707683.125</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1305260</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>906505.125</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>374579</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>275522.25</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>120680.375</c:v>
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>464.1173847</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>491.867939699999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>517.78979189999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>518.49335429999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>454.9267845</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>347.72126400000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>241.49296530000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99.787845599999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>73.399127399999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.149251900000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1FA6-43D9-8641-4895429DF0A7}"/>
+              <c16:uniqueId val="{00000002-EAEE-4C7D-BF3B-696838ED774A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -357,13 +485,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="182"/>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="583245408"/>
-        <c:axId val="583243112"/>
+        <c:axId val="485445656"/>
+        <c:axId val="485443032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="583245408"/>
+        <c:axId val="485445656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,7 +534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="583243112"/>
+        <c:crossAx val="485443032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -414,7 +542,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="583243112"/>
+        <c:axId val="485443032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,7 +593,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="583245408"/>
+        <c:crossAx val="485445656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -479,7 +607,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -561,7 +688,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -603,11 +729,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>prediction</c:v>
+                  <c:v>prediction_kbps</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -624,49 +750,49 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$42:$A$45</c:f>
+              <c:f>Sheet1!$B$8:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$5</c:f>
+              <c:f>Sheet1!$D$8:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5542941.625</c:v>
+                  <c:v>1476.6396489000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1483772.25</c:v>
+                  <c:v>395.27692739999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>811175.125</c:v>
+                  <c:v>216.0970533</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>603595</c:v>
+                  <c:v>160.797708</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-56A4-4D69-9EFC-91947BD6E695}"/>
+              <c16:uniqueId val="{00000000-75CE-4E5E-B8D1-19EDCEB5A5CA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -675,11 +801,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>residual</c:v>
+                  <c:v>residual_kbps</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -696,49 +822,49 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$42:$A$45</c:f>
+              <c:f>Sheet1!$B$8:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$5</c:f>
+              <c:f>Sheet1!$E$8:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11813752.25</c:v>
+                  <c:v>3147.1835993999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1849526.75</c:v>
+                  <c:v>492.7139262</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>795704.625</c:v>
+                  <c:v>211.97571209999899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>381760.625</c:v>
+                  <c:v>101.7010305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-56A4-4D69-9EFC-91947BD6E695}"/>
+              <c16:uniqueId val="{00000001-75CE-4E5E-B8D1-19EDCEB5A5CA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -747,11 +873,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>other</c:v>
+                  <c:v>other_kbps</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -768,49 +894,49 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$42:$A$45</c:f>
+              <c:f>Sheet1!$B$8:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$5</c:f>
+              <c:f>Sheet1!$F$8:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>906505.125</c:v>
+                  <c:v>241.49296530000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>374579</c:v>
+                  <c:v>99.787845599999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>275522.25</c:v>
+                  <c:v>73.399127399999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120680.375</c:v>
+                  <c:v>32.149251900000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-56A4-4D69-9EFC-91947BD6E695}"/>
+              <c16:uniqueId val="{00000002-75CE-4E5E-B8D1-19EDCEB5A5CA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -824,11 +950,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="349940640"/>
-        <c:axId val="349940968"/>
+        <c:axId val="486875296"/>
+        <c:axId val="486876608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="349940640"/>
+        <c:axId val="486875296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -871,7 +997,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349940968"/>
+        <c:crossAx val="486876608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -879,7 +1005,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="349940968"/>
+        <c:axId val="486876608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,7 +1056,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349940640"/>
+        <c:crossAx val="486875296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -944,7 +1070,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1092,7 +1217,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2105,23 +2230,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A323DBCD-2D43-4B0B-9361-5FBE102B5354}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{714C7F7D-E20D-4915-B708-48D7659A6A13}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2141,20 +2266,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>585105</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>106134</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>244928</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>48985</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B25841E5-B020-4E5D-853C-6BD505B76118}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2469,21 +2600,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2496,223 +2632,295 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>363976743</v>
       </c>
       <c r="B2">
-        <v>21653017.5</v>
+        <v>100000</v>
       </c>
       <c r="C2">
-        <v>340581543.125</v>
+        <v>96963.404335200001</v>
       </c>
       <c r="D2">
-        <v>1742182.375</v>
+        <v>5768.3638620000002</v>
+      </c>
+      <c r="E2">
+        <v>90730.9230885</v>
       </c>
       <c r="F2">
-        <v>18263199</v>
+        <v>464.1173847</v>
       </c>
       <c r="G2">
-        <v>5542941.625</v>
+        <v>32.050589000000002</v>
       </c>
       <c r="H2">
-        <v>11813752.25</v>
-      </c>
-      <c r="I2">
-        <v>906505.125</v>
+        <v>6.29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>289970358</v>
       </c>
       <c r="B3">
-        <v>21864241.625</v>
+        <v>80000</v>
       </c>
       <c r="C3">
-        <v>266259765.25</v>
+        <v>77248.103371200006</v>
       </c>
       <c r="D3">
-        <v>1846351.125</v>
+        <v>5824.6339688999997</v>
+      </c>
+      <c r="E3">
+        <v>70931.601462599996</v>
       </c>
       <c r="F3">
-        <v>3707878</v>
+        <v>491.867939699999</v>
       </c>
       <c r="G3">
-        <v>1483772.25</v>
+        <v>32.047114999999998</v>
       </c>
       <c r="H3">
-        <v>1849526.75</v>
-      </c>
-      <c r="I3">
-        <v>374579</v>
+        <v>8.14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>217022706</v>
       </c>
       <c r="B4">
-        <v>20674481.75</v>
+        <v>60000</v>
       </c>
       <c r="C4">
-        <v>194404568.875</v>
+        <v>57814.8488784</v>
       </c>
       <c r="D4">
-        <v>1943655.375</v>
+        <v>5507.6819381999903</v>
+      </c>
+      <c r="E4">
+        <v>51789.377148300002</v>
       </c>
       <c r="F4">
-        <v>1882402</v>
+        <v>517.78979189999995</v>
       </c>
       <c r="G4">
-        <v>811175.125</v>
+        <v>32.045279999999998</v>
       </c>
       <c r="H4">
-        <v>795704.625</v>
-      </c>
-      <c r="I4">
-        <v>275522.25</v>
+        <v>10.32</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>144913374</v>
       </c>
       <c r="B5">
-        <v>17901690.5</v>
+        <v>40000</v>
       </c>
       <c r="C5">
-        <v>125065387.125</v>
+        <v>38604.922833600001</v>
       </c>
       <c r="D5">
-        <v>1946296.375</v>
+        <v>4769.0103491999998</v>
+      </c>
+      <c r="E5">
+        <v>33317.419130099901</v>
       </c>
       <c r="F5">
-        <v>1106036</v>
+        <v>518.49335429999996</v>
       </c>
       <c r="G5">
-        <v>603595</v>
+        <v>32.040278000000001</v>
       </c>
       <c r="H5">
-        <v>381760.625</v>
-      </c>
-      <c r="I5">
-        <v>120680.375</v>
+        <v>13.41</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>73105843</v>
       </c>
       <c r="B6">
-        <v>12995767</v>
+        <v>20000</v>
       </c>
       <c r="C6">
-        <v>58402392.875</v>
+        <v>19475.396575199899</v>
       </c>
       <c r="D6">
-        <v>1707683.125</v>
+        <v>3462.0723287999999</v>
+      </c>
+      <c r="E6">
+        <v>15558.3974619</v>
+      </c>
+      <c r="F6">
+        <v>454.9267845</v>
+      </c>
+      <c r="G6">
+        <v>32.014301000000003</v>
+      </c>
+      <c r="H6">
+        <v>18.79</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>36544663</v>
       </c>
       <c r="B7">
-        <v>8831983.125</v>
+        <v>10000</v>
       </c>
       <c r="C7">
-        <v>26407419.875</v>
+        <v>9735.4982232000002</v>
       </c>
       <c r="D7">
-        <v>1305260</v>
+        <v>2352.8403045</v>
+      </c>
+      <c r="E7">
+        <v>7034.9366547</v>
+      </c>
+      <c r="F7">
+        <v>347.72126400000002</v>
+      </c>
+      <c r="G7">
+        <v>31.947144999999999</v>
+      </c>
+      <c r="H7">
+        <v>24.47</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>18263199</v>
       </c>
       <c r="B8">
-        <v>5542941.625</v>
+        <v>5000</v>
       </c>
       <c r="C8">
-        <v>11813752.25</v>
+        <v>4865.3162136000001</v>
       </c>
       <c r="D8">
-        <v>906505.125</v>
+        <v>1476.6396489000001</v>
+      </c>
+      <c r="E8">
+        <v>3147.1835993999998</v>
+      </c>
+      <c r="F8">
+        <v>241.49296530000001</v>
+      </c>
+      <c r="G8">
+        <v>31.799208</v>
+      </c>
+      <c r="H8">
+        <v>30.41</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3707878</v>
       </c>
       <c r="B9">
-        <v>1483772.25</v>
+        <v>1000</v>
       </c>
       <c r="C9">
-        <v>1849526.75</v>
+        <v>987.77869920000001</v>
       </c>
       <c r="D9">
-        <v>374579</v>
+        <v>395.27692739999998</v>
+      </c>
+      <c r="E9">
+        <v>492.7139262</v>
+      </c>
+      <c r="F9">
+        <v>99.787845599999997</v>
+      </c>
+      <c r="G9">
+        <v>30.975273999999999</v>
+      </c>
+      <c r="H9">
+        <v>42.2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1882402</v>
       </c>
       <c r="B10">
-        <v>811175.125</v>
+        <v>500</v>
       </c>
       <c r="C10">
-        <v>795704.625</v>
+        <v>501.47189279999998</v>
       </c>
       <c r="D10">
-        <v>275522.25</v>
+        <v>216.0970533</v>
+      </c>
+      <c r="E10">
+        <v>211.97571209999899</v>
+      </c>
+      <c r="F10">
+        <v>73.399127399999998</v>
+      </c>
+      <c r="G10">
+        <v>30.377583000000001</v>
+      </c>
+      <c r="H10">
+        <v>46.64</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1106036</v>
       </c>
       <c r="B11">
-        <v>603595</v>
+        <v>250</v>
       </c>
       <c r="C11">
-        <v>381760.625</v>
+        <v>294.64799040000003</v>
       </c>
       <c r="D11">
-        <v>120680.375</v>
+        <v>160.797708</v>
+      </c>
+      <c r="E11">
+        <v>101.7010305</v>
+      </c>
+      <c r="F11">
+        <v>32.149251900000003</v>
+      </c>
+      <c r="G11">
+        <v>28.673165999999998</v>
+      </c>
+      <c r="H11">
+        <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>10</v>
       </c>

</xml_diff>